<commit_message>
add the benchmark models in /benchmark/
</commit_message>
<xml_diff>
--- a/doc/LW_XGBoost_Cloud.xlsx
+++ b/doc/LW_XGBoost_Cloud.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5f1e44f6614d5618/CODE/LW_XGBoost_Cloud/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="8_{BA299217-D0CE-704C-8DB3-9D9BE35E2107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{903E6381-C220-E54C-8F0F-982736047F2D}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="8_{BA299217-D0CE-704C-8DB3-9D9BE35E2107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C0A567C-2821-6345-BF30-1D07729484D6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{CFBFBA78-76F9-8847-BDA4-A80AE4F10A0C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="1" xr2:uid="{CFBFBA78-76F9-8847-BDA4-A80AE4F10A0C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="inputs" sheetId="1" r:id="rId1"/>
+    <sheet name="model selection" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_Hlk113521170" localSheetId="0">Sheet1!$D$10</definedName>
-    <definedName name="_Hlk113521253" localSheetId="0">Sheet1!$D$9</definedName>
-    <definedName name="OLE_LINK12" localSheetId="0">Sheet1!$G$13</definedName>
+    <definedName name="_Hlk113521170" localSheetId="0">inputs!$D$10</definedName>
+    <definedName name="_Hlk113521253" localSheetId="0">inputs!$D$9</definedName>
+    <definedName name="OLE_LINK12" localSheetId="0">inputs!$G$13</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="60">
   <si>
     <t>Variable</t>
   </si>
@@ -161,13 +162,73 @@
   </si>
   <si>
     <t>(CGR4 pyrgeometer)</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Training Time</t>
+  </si>
+  <si>
+    <t>Inference Time</t>
+  </si>
+  <si>
+    <t>MAE</t>
+  </si>
+  <si>
+    <t>MSE</t>
+  </si>
+  <si>
+    <t>RMSE</t>
+  </si>
+  <si>
+    <t>R² (R-Squared)</t>
+  </si>
+  <si>
+    <t>Interpretability</t>
+  </si>
+  <si>
+    <t>Robustness to Outliers</t>
+  </si>
+  <si>
+    <t>XGBoost Regressor</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Linear Regression</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Ridge Regression</t>
+  </si>
+  <si>
+    <t>Lasso Regression</t>
+  </si>
+  <si>
+    <t>Random Forest Regressor</t>
+  </si>
+  <si>
+    <t>Gradient Boosting Regressor</t>
+  </si>
+  <si>
+    <t>Support Vector Regressor</t>
+  </si>
+  <si>
+    <t>Neural Network Regressor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -188,6 +249,21 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -197,12 +273,142 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -212,22 +418,7 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="double">
         <color indexed="64"/>
       </bottom>
@@ -238,9 +429,7 @@
         <color rgb="FF000000"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="double">
         <color indexed="64"/>
       </bottom>
@@ -251,132 +440,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="double">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -389,20 +453,9 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -410,71 +463,66 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -482,17 +530,268 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="double">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="double">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -505,10 +804,25 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A2294B34-A7A6-9C41-B02C-C554CCB28E5B}" name="Table1" displayName="Table1" ref="D9:I25" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="7" tableBorderDxfId="8">
+  <autoFilter ref="D9:I25" xr:uid="{A2294B34-A7A6-9C41-B02C-C554CCB28E5B}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{476E816E-5A6A-604E-9FD5-DB0682FC20BE}" name="Variable" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{DF2F0ADD-7818-6448-8759-929905EF8C3E}" name="Full name" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{6D56A426-61DA-C343-B5CE-38DC7411B41A}" name="unit" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{BF8F5922-6003-C441-82B3-11D351B33A36}" name="data source (device)" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{DBEEDB4B-EB5A-644C-8538-2266E5B8F2BE}" name="XGBoost" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{CB282794-EAFD-B740-85F3-F326D49B051E}" name="APACADA" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -546,7 +860,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -652,7 +966,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -794,7 +1108,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -802,327 +1116,473 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B781742-D24E-2244-8D4E-B041E241801C}">
-  <dimension ref="D9:I26"/>
+  <dimension ref="D9:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C8" zoomScale="340" zoomScaleNormal="340" workbookViewId="0">
-      <selection activeCell="I24" sqref="D9:I25"/>
+    <sheetView topLeftCell="C14" zoomScale="142" zoomScaleNormal="340" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="7.33203125" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" customWidth="1"/>
     <col min="5" max="5" width="19.1640625" customWidth="1"/>
     <col min="6" max="6" width="6" customWidth="1"/>
     <col min="7" max="7" width="23.83203125" customWidth="1"/>
-    <col min="8" max="8" width="8.5" customWidth="1"/>
-    <col min="9" max="9" width="9.5" customWidth="1"/>
+    <col min="8" max="8" width="9.5" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="9" spans="4:9" ht="31" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="4:9" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="17" t="s">
+    <row r="10" spans="4:9" ht="29" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="4:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D11" s="12"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="19" t="s">
+    <row r="11" spans="4:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D11" s="5"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="8"/>
-    </row>
-    <row r="12" spans="4:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="12" t="s">
+      <c r="H11" s="1"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="4:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="20" t="s">
+      <c r="G12" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="4:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D13" s="12"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="19" t="s">
+    <row r="13" spans="4:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="6"/>
-      <c r="I13" s="8"/>
-    </row>
-    <row r="14" spans="4:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D14" s="12" t="s">
+      <c r="H13" s="1"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="4:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="4:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D15" s="12"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="19" t="s">
+    <row r="15" spans="4:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D15" s="5"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="8"/>
-    </row>
-    <row r="16" spans="4:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D16" s="12" t="s">
+      <c r="H15" s="1"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="4:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D16" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G16" s="20" t="s">
+      <c r="G16" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="I16" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="4:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D17" s="12"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="19" t="s">
+    <row r="17" spans="4:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D17" s="5"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H17" s="6"/>
-      <c r="I17" s="8"/>
-    </row>
-    <row r="18" spans="4:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D18" s="12" t="s">
+      <c r="H17" s="1"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="4:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D18" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G18" s="20" t="s">
+      <c r="G18" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="H18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="I18" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="4:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D19" s="12"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="19" t="s">
+    <row r="19" spans="4:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D19" s="5"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="6"/>
-      <c r="I19" s="8"/>
-    </row>
-    <row r="20" spans="4:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D20" s="12" t="s">
+      <c r="H19" s="1"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="4:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="20" t="s">
+      <c r="G20" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I20" s="8" t="s">
+      <c r="I20" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="4:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D21" s="12"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="19" t="s">
+    <row r="21" spans="4:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D21" s="5"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="6"/>
-      <c r="I21" s="8"/>
-    </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D22" s="12" t="s">
+      <c r="H21" s="1"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="4:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D22" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G22" s="20" t="s">
+      <c r="G22" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H22" s="6" t="s">
+      <c r="H22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="I22" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="4:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="D23" s="12"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="19" t="s">
+    <row r="23" spans="4:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D23" s="5"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="H23" s="6"/>
-      <c r="I23" s="8"/>
-    </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D24" s="12" t="s">
+      <c r="H23" s="1"/>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="4:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D24" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E24" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G24" s="20" t="s">
+      <c r="G24" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="H24" s="6" t="s">
+      <c r="H24" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I24" s="8" t="s">
+      <c r="I24" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="4:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D25" s="13"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="21" t="s">
+    <row r="25" spans="4:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D25" s="17"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="H25" s="7"/>
-      <c r="I25" s="9"/>
-    </row>
-    <row r="26" spans="4:9" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="20"/>
+    </row>
   </sheetData>
-  <mergeCells count="40">
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="I22:I23"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37DDB6CF-8512-D146-9DCA-B9E4D6E44482}">
+  <dimension ref="D5:L13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="15.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D5" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="L5" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D6" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D7" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="L7" s="22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D8" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="L8" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D9" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="L9" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D10" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="L10" s="22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D11" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="L11" s="22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D12" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="L12" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D13" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="L13" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add RF model trained, tested. backup GPU version XGB
</commit_message>
<xml_diff>
--- a/doc/LW_XGBoost_Cloud.xlsx
+++ b/doc/LW_XGBoost_Cloud.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5f1e44f6614d5618/CODE/LW_XGBoost_Cloud/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="8_{BA299217-D0CE-704C-8DB3-9D9BE35E2107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C0A567C-2821-6345-BF30-1D07729484D6}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="8_{BA299217-D0CE-704C-8DB3-9D9BE35E2107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CEB2460-6B42-3946-AAD9-0BC042E0A5FB}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="1" xr2:uid="{CFBFBA78-76F9-8847-BDA4-A80AE4F10A0C}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_Hlk113521253" localSheetId="0">inputs!$D$9</definedName>
     <definedName name="OLE_LINK12" localSheetId="0">inputs!$G$13</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="61">
   <si>
     <t>Variable</t>
   </si>
@@ -176,9 +176,6 @@
     <t>MAE</t>
   </si>
   <si>
-    <t>MSE</t>
-  </si>
-  <si>
     <t>RMSE</t>
   </si>
   <si>
@@ -191,9 +188,6 @@
     <t>Robustness to Outliers</t>
   </si>
   <si>
-    <t>XGBoost Regressor</t>
-  </si>
-  <si>
     <t>Medium</t>
   </si>
   <si>
@@ -222,6 +216,15 @@
   </si>
   <si>
     <t>Neural Network Regressor</t>
+  </si>
+  <si>
+    <t>XGBoost Regressor default</t>
+  </si>
+  <si>
+    <t>XGBoost Regressor tuned</t>
+  </si>
+  <si>
+    <t>COR</t>
   </si>
 </sst>
 </file>
@@ -542,7 +545,424 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="double">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="double">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -572,225 +992,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="double">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="double">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -805,17 +1006,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A2294B34-A7A6-9C41-B02C-C554CCB28E5B}" name="Table1" displayName="Table1" ref="D9:I25" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="7" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A2294B34-A7A6-9C41-B02C-C554CCB28E5B}" name="Table1" displayName="Table1" ref="D9:I25" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17">
   <autoFilter ref="D9:I25" xr:uid="{A2294B34-A7A6-9C41-B02C-C554CCB28E5B}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{476E816E-5A6A-604E-9FD5-DB0682FC20BE}" name="Variable" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{DF2F0ADD-7818-6448-8759-929905EF8C3E}" name="Full name" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{6D56A426-61DA-C343-B5CE-38DC7411B41A}" name="unit" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{BF8F5922-6003-C441-82B3-11D351B33A36}" name="data source (device)" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{DBEEDB4B-EB5A-644C-8538-2266E5B8F2BE}" name="XGBoost" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{CB282794-EAFD-B740-85F3-F326D49B051E}" name="APACADA" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{476E816E-5A6A-604E-9FD5-DB0682FC20BE}" name="Variable" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{DF2F0ADD-7818-6448-8759-929905EF8C3E}" name="Full name" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{6D56A426-61DA-C343-B5CE-38DC7411B41A}" name="unit" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{BF8F5922-6003-C441-82B3-11D351B33A36}" name="data source (device)" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{DBEEDB4B-EB5A-644C-8538-2266E5B8F2BE}" name="XGBoost" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{CB282794-EAFD-B740-85F3-F326D49B051E}" name="APACADA" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9EEF2A3D-F1E8-3D44-BA88-4B8DB480C99C}" name="Table2" displayName="Table2" ref="D5:L15" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="D5:L15" xr:uid="{9EEF2A3D-F1E8-3D44-BA88-4B8DB480C99C}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{D74C813E-BB13-9E4C-BE1B-5A25FFB3863F}" name="Model" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{1CBA73F1-E8D0-EA41-8C00-09B6E8A111C8}" name="MAE" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{E31586EE-562A-1246-9AB8-927E698C240B}" name="RMSE" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{1DC40ECE-13FC-7446-81AF-30A80D7276F6}" name="COR" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{295D2A06-3377-5840-94A4-39451AAB1A52}" name="R² (R-Squared)" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{EB2838EC-7A49-E945-AA3B-B7A722A935A1}" name="Training Time" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{B3C093B6-EA73-AE47-A2EE-F6039F684554}" name="Inference Time" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{F464B0C7-7363-A042-836C-9AF6A7FE72D8}" name="Interpretability" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{B449C696-EE9C-D147-AFEB-30DB94C536A2}" name="Robustness to Outliers" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1403,18 +1622,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37DDB6CF-8512-D146-9DCA-B9E4D6E44482}">
-  <dimension ref="D5:L13"/>
+  <dimension ref="D5:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="26.1640625" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" customWidth="1"/>
-    <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="15.1640625" customWidth="1"/>
+    <col min="5" max="7" width="7.33203125" customWidth="1"/>
+    <col min="8" max="10" width="15.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.5" customWidth="1"/>
+    <col min="12" max="12" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="4:12" x14ac:dyDescent="0.2">
@@ -1428,10 +1648,10 @@
         <v>44</v>
       </c>
       <c r="G5" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="21" t="s">
         <v>45</v>
-      </c>
-      <c r="H5" s="21" t="s">
-        <v>46</v>
       </c>
       <c r="I5" s="21" t="s">
         <v>41</v>
@@ -1440,66 +1660,72 @@
         <v>42</v>
       </c>
       <c r="K5" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" s="21" t="s">
         <v>47</v>
-      </c>
-      <c r="L5" s="21" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="6" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D6" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="22"/>
+        <v>59</v>
+      </c>
+      <c r="E6" s="22">
+        <v>1</v>
+      </c>
       <c r="F6" s="22"/>
       <c r="G6" s="22"/>
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
       <c r="J6" s="22"/>
       <c r="K6" s="22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L6" s="22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D7" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="22"/>
+        <v>58</v>
+      </c>
+      <c r="E7" s="22">
+        <v>1</v>
+      </c>
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
       <c r="K7" s="22" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D8" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="22"/>
+        <v>50</v>
+      </c>
+      <c r="E8" s="22">
+        <v>0</v>
+      </c>
       <c r="F8" s="22"/>
       <c r="G8" s="22"/>
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
       <c r="J8" s="22"/>
       <c r="K8" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="L8" s="22" t="s">
         <v>51</v>
-      </c>
-      <c r="L8" s="22" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="9" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D9" s="21" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
@@ -1508,15 +1734,15 @@
       <c r="I9" s="22"/>
       <c r="J9" s="22"/>
       <c r="K9" s="22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L9" s="22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D10" s="21" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
@@ -1525,32 +1751,34 @@
       <c r="I10" s="22"/>
       <c r="J10" s="22"/>
       <c r="K10" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L10" s="22" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D11" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="22"/>
+        <v>54</v>
+      </c>
+      <c r="E11" s="22">
+        <v>1</v>
+      </c>
       <c r="F11" s="22"/>
       <c r="G11" s="22"/>
       <c r="H11" s="22"/>
       <c r="I11" s="22"/>
       <c r="J11" s="22"/>
       <c r="K11" s="22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D12" s="21" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
@@ -1559,30 +1787,54 @@
       <c r="I12" s="22"/>
       <c r="J12" s="22"/>
       <c r="K12" s="22" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="L12" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D13" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="E13" s="22"/>
+        <v>56</v>
+      </c>
+      <c r="E13" s="22">
+        <v>0</v>
+      </c>
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
       <c r="H13" s="22"/>
       <c r="I13" s="22"/>
       <c r="J13" s="22"/>
       <c r="K13" s="22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L13" s="22" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D14" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="22">
+        <v>1</v>
+      </c>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="L14" s="22" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
using 5-min data.model update
</commit_message>
<xml_diff>
--- a/doc/LW_XGBoost_Cloud.xlsx
+++ b/doc/LW_XGBoost_Cloud.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5f1e44f6614d5618/CODE/LW_XGBoost_Cloud/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="8_{BA299217-D0CE-704C-8DB3-9D9BE35E2107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CEB2460-6B42-3946-AAD9-0BC042E0A5FB}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="8_{BA299217-D0CE-704C-8DB3-9D9BE35E2107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B02414B5-B602-7846-9E28-A27CAB6121E5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="1" xr2:uid="{CFBFBA78-76F9-8847-BDA4-A80AE4F10A0C}"/>
+    <workbookView xWindow="-40600" yWindow="6000" windowWidth="28800" windowHeight="16260" activeTab="1" xr2:uid="{CFBFBA78-76F9-8847-BDA4-A80AE4F10A0C}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs" sheetId="1" r:id="rId1"/>
@@ -1625,7 +1625,7 @@
   <dimension ref="D5:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C12" sqref="A12:XFD12"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1671,11 +1671,17 @@
         <v>59</v>
       </c>
       <c r="E6" s="22">
-        <v>1</v>
-      </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F6" s="22">
+        <v>0.1</v>
+      </c>
+      <c r="G6" s="22">
+        <v>0.92</v>
+      </c>
+      <c r="H6" s="22">
+        <v>0.84</v>
+      </c>
       <c r="I6" s="22"/>
       <c r="J6" s="22"/>
       <c r="K6" s="22" t="s">
@@ -1690,11 +1696,17 @@
         <v>58</v>
       </c>
       <c r="E7" s="22">
-        <v>1</v>
-      </c>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
+        <v>0.08</v>
+      </c>
+      <c r="F7" s="22">
+        <v>0.11</v>
+      </c>
+      <c r="G7" s="22">
+        <v>0.91</v>
+      </c>
+      <c r="H7" s="22">
+        <v>0.82</v>
+      </c>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
       <c r="K7" s="22" t="s">
@@ -1708,9 +1720,7 @@
       <c r="D8" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="22">
-        <v>0</v>
-      </c>
+      <c r="E8" s="22"/>
       <c r="F8" s="22"/>
       <c r="G8" s="22"/>
       <c r="H8" s="22"/>
@@ -1762,11 +1772,17 @@
         <v>54</v>
       </c>
       <c r="E11" s="22">
-        <v>1</v>
-      </c>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F11" s="22">
+        <v>0.11</v>
+      </c>
+      <c r="G11" s="22">
+        <v>0.92</v>
+      </c>
+      <c r="H11" s="22">
+        <v>0.83</v>
+      </c>
       <c r="I11" s="22"/>
       <c r="J11" s="22"/>
       <c r="K11" s="22" t="s">
@@ -1797,9 +1813,7 @@
       <c r="D13" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="E13" s="22">
-        <v>0</v>
-      </c>
+      <c r="E13" s="22"/>
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
       <c r="H13" s="22"/>
@@ -1817,11 +1831,17 @@
         <v>57</v>
       </c>
       <c r="E14" s="22">
-        <v>1</v>
-      </c>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
+        <v>0.09</v>
+      </c>
+      <c r="F14" s="22">
+        <v>0.13</v>
+      </c>
+      <c r="G14" s="22">
+        <v>0.87</v>
+      </c>
+      <c r="H14" s="22">
+        <v>0.73</v>
+      </c>
       <c r="I14" s="22"/>
       <c r="J14" s="22"/>
       <c r="K14" s="22" t="s">

</xml_diff>